<commit_message>
Use Cases and Functional Requirements
</commit_message>
<xml_diff>
--- a/design/Functional Requirements Matrix.xlsx
+++ b/design/Functional Requirements Matrix.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
   <si>
     <t>Brewer              Buddy</t>
   </si>
@@ -2310,10 +2310,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ23"/>
+  <dimension ref="A1:AJ26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2734,12 +2734,22 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
       <c r="Y9" s="9"/>
@@ -2814,7 +2824,9 @@
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
+      <c r="Q11" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
       <c r="T11" s="9"/>
@@ -3295,7 +3307,7 @@
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
-      <c r="N23" s="8"/>
+      <c r="N23" s="9"/>
       <c r="O23" s="8" t="s">
         <v>23</v>
       </c>
@@ -3321,11 +3333,135 @@
       <c r="AI23" s="9"/>
       <c r="AJ23" s="9"/>
     </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>41</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="9"/>
+      <c r="AJ24" s="9"/>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>42</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="9"/>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="9"/>
+      <c r="AJ25" s="9"/>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>43</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
+      <c r="AG26" s="9"/>
+      <c r="AH26" s="9"/>
+      <c r="AI26" s="9"/>
+      <c r="AJ26" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C2:AJ2"/>
-    <mergeCell ref="B3:B23"/>
+    <mergeCell ref="B3:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>